<commit_message>
v1.8.9.7: more autoRotateBack at higher speed
</commit_message>
<xml_diff>
--- a/Documents/parameter.xlsx
+++ b/Documents/parameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22560" yWindow="0" windowWidth="2520" windowHeight="9720"/>
+    <workbookView xWindow="25680" yWindow="0" windowWidth="2520" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -238,16 +238,16 @@
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -323,19 +323,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,10 +420,10 @@
                   <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.7</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -499,19 +499,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95</c:v>
+                  <c:v>1.0555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.84</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13999999999999999</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -526,11 +526,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="388544232"/>
-        <c:axId val="388544624"/>
+        <c:axId val="357006968"/>
+        <c:axId val="357007360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="388544232"/>
+        <c:axId val="357006968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -588,12 +588,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388544624"/>
+        <c:crossAx val="357007360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="388544624"/>
+        <c:axId val="357007360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -651,7 +651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="388544232"/>
+        <c:crossAx val="357006968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
@@ -1618,7 +1618,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F27"/>
+      <selection activeCell="F8" sqref="F8:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,16 +1655,16 @@
         <v>0.2</v>
       </c>
       <c r="C2">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="E2">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="F2">
-        <v>1.4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1672,19 +1672,20 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D3">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E3">
         <v>0.6</v>
       </c>
       <c r="F3">
-        <v>0.25</v>
+        <f>0.2/1.25</f>
+        <v>0.16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1701,10 +1702,10 @@
         <v>0.95</v>
       </c>
       <c r="E4">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1712,24 +1713,24 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f>B4*B2</f>
-        <v>0.2</v>
+        <f>B4/B3</f>
+        <v>0.5</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:F5" si="0">C4*C2</f>
-        <v>0.8</v>
+        <f t="shared" ref="C5:F5" si="0">C4/C3</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.95</v>
+        <v>1.0555555555555556</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.84</v>
+        <v>1.25</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0.13999999999999999</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1925,11 +1926,11 @@
       </c>
       <c r="E14" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
       <c r="F14" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;autoRotateBackFx1 type="float" value="0.8"/&gt;</v>
+        <v xml:space="preserve"> &lt;autoRotateBackFx1 type="float" value="0.85"/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1951,11 +1952,11 @@
       </c>
       <c r="E15" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F15" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;autoRotateBackFx2 type="float" value="1"/&gt;</v>
+        <v xml:space="preserve"> &lt;autoRotateBackFx2 type="float" value="1.2"/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,11 +1978,11 @@
       </c>
       <c r="E16" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="F16" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;autoRotateBackFx3 type="float" value="1.2"/&gt;</v>
+        <v xml:space="preserve"> &lt;autoRotateBackFx3 type="float" value="1.6"/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2003,11 +2004,11 @@
       </c>
       <c r="E17" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;autoRotateBackFxMax type="float" value="1.4"/&gt;</v>
+        <v xml:space="preserve"> &lt;autoRotateBackFxMax type="float" value="2"/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2029,11 +2030,11 @@
       </c>
       <c r="E18" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;axisSideFx0 type="float" value="1.5"/&gt;</v>
+        <v xml:space="preserve"> &lt;axisSideFx0 type="float" value="2"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2055,11 +2056,11 @@
       </c>
       <c r="E19" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F19" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;axisSideFx1 type="float" value="1"/&gt;</v>
+        <v xml:space="preserve"> &lt;axisSideFx1 type="float" value="1.2"/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2081,11 +2082,11 @@
       </c>
       <c r="E20" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="F20" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;axisSideFx2 type="float" value="0.8"/&gt;</v>
+        <v xml:space="preserve"> &lt;axisSideFx2 type="float" value="0.9"/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2133,11 +2134,11 @@
       </c>
       <c r="E22" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>0.25</v>
+        <v>0.16</v>
       </c>
       <c r="F22" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;axisSideFxMax type="float" value="0.25"/&gt;</v>
+        <v xml:space="preserve"> &lt;axisSideFxMax type="float" value="0.16"/&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,11 +2238,11 @@
       </c>
       <c r="E26" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="F26" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;maxRotTimeFx3 type="float" value="0.7"/&gt;</v>
+        <v xml:space="preserve"> &lt;maxRotTimeFx3 type="float" value="0.75"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2263,11 +2264,11 @@
       </c>
       <c r="E27" s="2">
         <f>INDEX($B$1:$F$4,Table1[[#This Row],[column]]+1,Table1[[#This Row],[number]]+1)</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F27" s="2" t="str">
         <f>CONCATENATE(" &lt;",Table1[[#This Row],[tag]]," type=""float"" value=""",Table1[[#This Row],[value]],"""/&gt;")</f>
-        <v xml:space="preserve"> &lt;maxRotTimeFxMax type="float" value="0.1"/&gt;</v>
+        <v xml:space="preserve"> &lt;maxRotTimeFxMax type="float" value="0.2"/&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>